<commit_message>
added some note to XLOOKUP
</commit_message>
<xml_diff>
--- a/air-routes-sfo.xlsx
+++ b/air-routes-sfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\youse\Desktop\Excel Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32169CD7-96E6-4DCC-89F8-CC484E57477E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFE3A163-1013-4161-8C5A-7345CAA57F93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4111" uniqueCount="3257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4112" uniqueCount="3258">
   <si>
     <t>ABE</t>
   </si>
@@ -9841,6 +9841,9 @@
   </si>
   <si>
     <t>from the pivot table in Pivot table sheet page we can see that United airlines is the most airline and the second one is Virgin America</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in this dataset we have applied the function XLOOKUP to merge the data from Airlines and Airports sheets with matched column of Airline check the formulas written in D and E columns </t>
   </si>
 </sst>
 </file>
@@ -11847,7 +11850,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{221D59D3-DD05-48F5-84E0-3AFD1B032C46}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{221D59D3-DD05-48F5-84E0-3AFD1B032C46}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B47" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField showAll="0">
@@ -12757,7 +12760,7 @@
   <dimension ref="A1:G250"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F15:F16"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -12985,7 +12988,7 @@
         <v>Avianca</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>2350</v>
       </c>
@@ -13002,6 +13005,9 @@
       <c r="E10" s="1" t="str">
         <f>_xlfn.XLOOKUP(C10,Airports!A:A,Airports!B:B)</f>
         <v>Chicago O'hare International Airport</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>3257</v>
       </c>
       <c r="G10" s="1" t="str">
         <v>Finnair</v>

</xml_diff>